<commit_message>
feat: Add luar daerah count to Dashboard and update EventPage with reload functionality
- Implemented luar daerah count in Dashboard component to track members outside the region.
- Enhanced EventPage with a reload button to refresh participant data.
- Updated PendingMembersTable and PendingAttendancesTable to display members from outside the region.
- Refactored card components in EventPage for cleaner UI.
- Added EventTimeline component to visualize member event history.
- Created MemberDetailPage to show detailed member information and event participation.
- Improved GeneralSettings and importPage for better user experience and clarity.
</commit_message>
<xml_diff>
--- a/public/template-impor-member.xlsx
+++ b/public/template-impor-member.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="member" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="template_impor" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -29,12 +29,20 @@
   </si>
   <si>
     <t>event_date</t>
+  </si>
+  <si>
+    <t>is_outside_region</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="mm.yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="166" formatCode="m.yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -45,6 +53,7 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,12 +70,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -303,6 +324,122 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" s="2"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="D3" s="2"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="D5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="2"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="D8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="D9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="D10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="D11" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="D12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="4"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="D14" s="5"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="5"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="2"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="2"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="2"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="2"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="2"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="2"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="2"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="D23" s="2"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="2"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="2"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" ht="16.5" customHeight="1">
+      <c r="D26" s="2"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="D28" s="4"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30">
+      <c r="D30" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>